<commit_message>
clean up files. Related but current stuff in background; old stuff in archive
</commit_message>
<xml_diff>
--- a/examples/GEOME/GEOMEFieldsAndMapping.xlsx
+++ b/examples/GEOME/GEOMEFieldsAndMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\examples\GEOME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025C0D74-7474-49EC-A462-513227F86E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D3F5FC-C20E-4CD7-BFC0-3EFC21C42C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="390" windowWidth="19590" windowHeight="11010" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1575" yWindow="3045" windowWidth="25725" windowHeight="13125" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllFieldsbyProject" sheetId="1" r:id="rId1"/>
@@ -29199,7 +29199,7 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" ref="E2:E33" si="0">IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
@@ -29215,7 +29215,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A3,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29231,7 +29231,7 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A4,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29247,7 +29247,7 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A5,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29263,7 +29263,7 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A6,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29279,7 +29279,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A7,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29295,7 +29295,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A8,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29311,7 +29311,7 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A9,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29329,7 +29329,7 @@
         <v>337</v>
       </c>
       <c r="E10" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A10,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29345,7 +29345,7 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A11,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29361,7 +29361,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A12,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29377,7 +29377,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A13,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29395,7 +29395,7 @@
         <v>386</v>
       </c>
       <c r="E14" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A14,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -29413,7 +29413,7 @@
         <v>388</v>
       </c>
       <c r="E15" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A15,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29431,7 +29431,7 @@
         <v>337</v>
       </c>
       <c r="E16" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A16,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29447,7 +29447,7 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A17,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29463,7 +29463,7 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A18,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29479,7 +29479,7 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A19,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29495,7 +29495,7 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A20,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29511,7 +29511,7 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A21,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29527,7 +29527,7 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A22,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29543,7 +29543,7 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A23,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29561,7 +29561,7 @@
         <v>337</v>
       </c>
       <c r="E24" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A24,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29579,7 +29579,7 @@
         <v>337</v>
       </c>
       <c r="E25" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A25,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29595,7 +29595,7 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A26,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29611,7 +29611,7 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A27,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29629,7 +29629,7 @@
         <v>386</v>
       </c>
       <c r="E28" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A28,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29647,7 +29647,7 @@
         <v>402</v>
       </c>
       <c r="E29" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A29,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29663,7 +29663,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A30,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29681,7 +29681,7 @@
         <v>396</v>
       </c>
       <c r="E31" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A31,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29699,7 +29699,7 @@
         <v>407</v>
       </c>
       <c r="E32" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A32,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29717,7 +29717,7 @@
         <v>407</v>
       </c>
       <c r="E33" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A33,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -29735,7 +29735,7 @@
         <v>407</v>
       </c>
       <c r="E34" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" ref="E34:E65" si="1">IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
@@ -29753,7 +29753,7 @@
         <v>407</v>
       </c>
       <c r="E35" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A35,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29771,7 +29771,7 @@
         <v>407</v>
       </c>
       <c r="E36" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A36,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29789,7 +29789,7 @@
         <v>337</v>
       </c>
       <c r="E37" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A37,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29805,7 +29805,7 @@
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A38,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29821,7 +29821,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A39,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29839,7 +29839,7 @@
         <v>337</v>
       </c>
       <c r="E40" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A40,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29855,7 +29855,7 @@
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A41,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29873,7 +29873,7 @@
         <v>337</v>
       </c>
       <c r="E42" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A42,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29891,7 +29891,7 @@
         <v>337</v>
       </c>
       <c r="E43" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A43,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29907,7 +29907,7 @@
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A44,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29923,7 +29923,7 @@
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A45,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29939,7 +29939,7 @@
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A46,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29955,7 +29955,7 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A47,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29971,7 +29971,7 @@
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A48,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -29989,7 +29989,7 @@
         <v>412</v>
       </c>
       <c r="E49" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A49,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30007,7 +30007,7 @@
         <v>412</v>
       </c>
       <c r="E50" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A50,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30025,7 +30025,7 @@
         <v>412</v>
       </c>
       <c r="E51" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A51,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30043,7 +30043,7 @@
         <v>412</v>
       </c>
       <c r="E52" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A52,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30061,7 +30061,7 @@
         <v>412</v>
       </c>
       <c r="E53" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A53,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30077,7 +30077,7 @@
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A54,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30093,11 +30093,11 @@
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A55,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>182</v>
       </c>
@@ -30109,11 +30109,11 @@
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A56,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>183</v>
       </c>
@@ -30125,11 +30125,11 @@
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A57,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>184</v>
       </c>
@@ -30143,11 +30143,11 @@
         <v>413</v>
       </c>
       <c r="E58" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A58,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>185</v>
       </c>
@@ -30159,11 +30159,11 @@
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A59,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>186</v>
       </c>
@@ -30177,7 +30177,7 @@
         <v>404</v>
       </c>
       <c r="E60" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A60,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30195,7 +30195,7 @@
         <v>404</v>
       </c>
       <c r="E61" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A61,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30213,7 +30213,7 @@
         <v>337</v>
       </c>
       <c r="E62" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A62,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30229,7 +30229,7 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A63,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30247,7 +30247,7 @@
         <v>337</v>
       </c>
       <c r="E64" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A64,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30265,7 +30265,7 @@
         <v>413</v>
       </c>
       <c r="E65" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A65,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -30281,7 +30281,7 @@
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A66,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" ref="E66:E82" si="2">IF(ISERROR(VLOOKUP(A66,column_name,1,FALSE)),FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
@@ -30299,7 +30299,7 @@
         <v>404</v>
       </c>
       <c r="E67" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A67,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30317,7 +30317,7 @@
         <v>404</v>
       </c>
       <c r="E68" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A68,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30335,7 +30335,7 @@
         <v>386</v>
       </c>
       <c r="E69" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A69,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30351,7 +30351,7 @@
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A70,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30367,7 +30367,7 @@
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A71,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30383,7 +30383,7 @@
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A72,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30401,7 +30401,7 @@
         <v>337</v>
       </c>
       <c r="E73" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A73,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30417,7 +30417,7 @@
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A74,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30435,7 +30435,7 @@
         <v>398</v>
       </c>
       <c r="E75" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A75,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30453,7 +30453,7 @@
         <v>406</v>
       </c>
       <c r="E76" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A76,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30469,7 +30469,7 @@
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A77,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30485,7 +30485,7 @@
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A78,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30503,7 +30503,7 @@
         <v>403</v>
       </c>
       <c r="E79" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A79,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30519,7 +30519,7 @@
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A80,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30535,7 +30535,7 @@
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A81,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30551,7 +30551,7 @@
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A82,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -30579,7 +30579,7 @@
   <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -30624,7 +30624,7 @@
         <v>416</v>
       </c>
       <c r="E2" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" ref="E2:E33" si="0">IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
         <v>1</v>
       </c>
     </row>
@@ -30642,7 +30642,7 @@
         <v>417</v>
       </c>
       <c r="E3" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A3,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30660,7 +30660,7 @@
         <v>418</v>
       </c>
       <c r="E4" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A4,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30678,7 +30678,7 @@
         <v>423</v>
       </c>
       <c r="E5" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A5,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30694,7 +30694,7 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A6,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30712,7 +30712,7 @@
         <v>420</v>
       </c>
       <c r="E7" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A7,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30728,7 +30728,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A8,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30744,7 +30744,7 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A9,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30762,7 +30762,7 @@
         <v>418</v>
       </c>
       <c r="E10" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A10,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30780,7 +30780,7 @@
         <v>418</v>
       </c>
       <c r="E11" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A11,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30796,7 +30796,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A12,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -30814,7 +30814,7 @@
         <v>428</v>
       </c>
       <c r="E13" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A13,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30832,7 +30832,7 @@
         <v>428</v>
       </c>
       <c r="E14" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A14,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30850,7 +30850,7 @@
         <v>428</v>
       </c>
       <c r="E15" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A15,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30868,7 +30868,7 @@
         <v>430</v>
       </c>
       <c r="E16" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A16,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30886,7 +30886,7 @@
         <v>430</v>
       </c>
       <c r="E17" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A17,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30902,7 +30902,7 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A18,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30918,7 +30918,7 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A19,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30934,7 +30934,7 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A20,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30946,7 +30946,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A21,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30962,7 +30962,7 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A22,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30980,7 +30980,7 @@
         <v>432</v>
       </c>
       <c r="E23" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A23,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -30996,7 +30996,7 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A24,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31012,7 +31012,7 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A25,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31028,7 +31028,7 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A26,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31044,7 +31044,7 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A27,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31058,7 +31058,7 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A28,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31074,7 +31074,7 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A29,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31090,7 +31090,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A30,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31106,7 +31106,7 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A31,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31122,7 +31122,7 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A32,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31138,7 +31138,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A33,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -31154,7 +31154,7 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" ref="E34:E65" si="1">IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
@@ -31170,7 +31170,7 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A35,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31186,7 +31186,7 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A36,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31202,7 +31202,7 @@
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A37,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31218,7 +31218,7 @@
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A38,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31234,7 +31234,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A39,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31250,7 +31250,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A40,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31266,7 +31266,7 @@
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A41,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31282,7 +31282,7 @@
         <v>441</v>
       </c>
       <c r="E42" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A42,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31298,7 +31298,7 @@
         <v>441</v>
       </c>
       <c r="E43" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A43,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31314,7 +31314,7 @@
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A44,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31330,7 +31330,7 @@
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A45,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31346,7 +31346,7 @@
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A46,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31362,7 +31362,7 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A47,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31378,7 +31378,7 @@
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A48,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31394,7 +31394,7 @@
         <v>443</v>
       </c>
       <c r="E49" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A49,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31410,7 +31410,7 @@
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A50,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31426,7 +31426,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A51,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31442,7 +31442,7 @@
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A52,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31458,7 +31458,7 @@
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A53,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31474,7 +31474,7 @@
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A54,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31490,7 +31490,7 @@
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A55,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31506,7 +31506,7 @@
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A56,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31522,7 +31522,7 @@
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A57,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31538,7 +31538,7 @@
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A58,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31554,7 +31554,7 @@
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A59,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31570,7 +31570,7 @@
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A60,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31586,7 +31586,7 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A61,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31602,7 +31602,7 @@
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A62,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31618,7 +31618,7 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A63,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31634,7 +31634,7 @@
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A64,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31650,7 +31650,7 @@
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A65,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -31666,7 +31666,7 @@
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A66,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" ref="E66:E84" si="2">IF(ISERROR(VLOOKUP(A66,column_name,1,FALSE)),FALSE,TRUE)</f>
         <v>0</v>
       </c>
     </row>
@@ -31682,7 +31682,7 @@
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A67,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31698,7 +31698,7 @@
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A68,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31714,7 +31714,7 @@
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A69,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31730,7 +31730,7 @@
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A70,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31746,7 +31746,7 @@
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A71,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31762,7 +31762,7 @@
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A72,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31778,7 +31778,7 @@
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A73,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31794,7 +31794,7 @@
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A74,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31810,7 +31810,7 @@
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A75,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31826,7 +31826,7 @@
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A76,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31844,7 +31844,7 @@
         <v>358</v>
       </c>
       <c r="E77" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A77,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31860,7 +31860,7 @@
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A78,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31876,7 +31876,7 @@
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A79,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31892,7 +31892,7 @@
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A80,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31908,7 +31908,7 @@
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A81,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31924,7 +31924,7 @@
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A82,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -31940,11 +31940,11 @@
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A83,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>279</v>
       </c>
@@ -31956,7 +31956,7 @@
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="b">
-        <f>IF(ISERROR(VLOOKUP(A84,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -32482,7 +32482,7 @@
     <sortCondition ref="A2:A21"/>
   </sortState>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>E2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32934,10 +32934,10 @@
     <sortCondition ref="A2:A34"/>
   </sortState>
   <conditionalFormatting sqref="A2:A34">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>E2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>E1048546</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>